<commit_message>
Corrélation r trouvée avec =PEARSON(matrice1;matrice2) et graphiques avec regression linéaire
</commit_message>
<xml_diff>
--- a/T2.xlsx
+++ b/T2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40c36b59fd529ece/Documents/Automne2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40c36b59fd529ece/Documents/Automne2023/IFT3913-TP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96496CC4-0BE0-4A13-AE07-BD2B45A3C171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{96496CC4-0BE0-4A13-AE07-BD2B45A3C171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C638F243-9FD4-49A1-A8D7-BEA6E7D8CCF7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{68C9A14E-2DFE-45A5-B2F7-CFC5049FF34D}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="358">
   <si>
     <t>class</t>
   </si>
@@ -1117,6 +1117,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>:TLOC et TASSERT</t>
+  </si>
+  <si>
+    <t>:WMC et TASSERT</t>
   </si>
 </sst>
 </file>
@@ -1152,9 +1158,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7784,7 +7789,7 @@
   <dimension ref="A1:G352"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7810,7 +7815,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
@@ -7826,9 +7831,12 @@
         <f>PEARSON(B1:B352,D1:D352)</f>
         <v>0.93957231879730008</v>
       </c>
+      <c r="G2" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
@@ -7845,7 +7853,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
@@ -7859,7 +7867,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
@@ -7875,9 +7883,12 @@
         <f>PEARSON(C1:C352,D1:D352)</f>
         <v>0.79247282652315254</v>
       </c>
+      <c r="G5" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
@@ -7891,7 +7902,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
@@ -7905,7 +7916,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
@@ -7919,7 +7930,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
@@ -7933,7 +7944,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
@@ -7947,7 +7958,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
@@ -7961,7 +7972,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
@@ -7975,7 +7986,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
@@ -7989,7 +8000,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
@@ -8003,7 +8014,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15">
@@ -8017,7 +8028,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16">
@@ -8031,7 +8042,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17">
@@ -8045,7 +8056,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18">
@@ -8059,7 +8070,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19">
@@ -8073,7 +8084,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20">
@@ -8087,7 +8098,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21">
@@ -8101,7 +8112,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22">
@@ -8115,7 +8126,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23">
@@ -8129,7 +8140,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24">
@@ -8143,7 +8154,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25">
@@ -8157,7 +8168,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
       <c r="B26">
@@ -8171,7 +8182,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27">
@@ -8185,7 +8196,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28">
@@ -8199,7 +8210,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29">
@@ -8213,7 +8224,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30">
@@ -8227,7 +8238,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>33</v>
       </c>
       <c r="B31">
@@ -8241,7 +8252,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>34</v>
       </c>
       <c r="B32">
@@ -8255,7 +8266,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33">
@@ -8269,7 +8280,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34">
@@ -8283,7 +8294,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>37</v>
       </c>
       <c r="B35">
@@ -8297,7 +8308,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>38</v>
       </c>
       <c r="B36">
@@ -8311,7 +8322,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>39</v>
       </c>
       <c r="B37">
@@ -8325,7 +8336,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>40</v>
       </c>
       <c r="B38">
@@ -8339,7 +8350,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="B39">
@@ -8353,7 +8364,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>42</v>
       </c>
       <c r="B40">
@@ -8367,7 +8378,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>43</v>
       </c>
       <c r="B41">
@@ -8381,7 +8392,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>44</v>
       </c>
       <c r="B42">
@@ -8395,7 +8406,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>45</v>
       </c>
       <c r="B43">
@@ -8409,7 +8420,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>46</v>
       </c>
       <c r="B44">
@@ -8423,7 +8434,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>47</v>
       </c>
       <c r="B45">
@@ -8437,7 +8448,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>48</v>
       </c>
       <c r="B46">
@@ -8451,7 +8462,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>49</v>
       </c>
       <c r="B47">
@@ -8465,7 +8476,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>50</v>
       </c>
       <c r="B48">
@@ -8479,7 +8490,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>51</v>
       </c>
       <c r="B49">
@@ -8493,7 +8504,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>52</v>
       </c>
       <c r="B50">
@@ -8507,7 +8518,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>53</v>
       </c>
       <c r="B51">
@@ -8521,7 +8532,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>54</v>
       </c>
       <c r="B52">
@@ -8535,7 +8546,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>55</v>
       </c>
       <c r="B53">
@@ -8549,7 +8560,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>56</v>
       </c>
       <c r="B54">
@@ -8563,7 +8574,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>57</v>
       </c>
       <c r="B55">
@@ -8577,7 +8588,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>58</v>
       </c>
       <c r="B56">
@@ -8591,7 +8602,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>59</v>
       </c>
       <c r="B57">
@@ -8605,7 +8616,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>60</v>
       </c>
       <c r="B58">
@@ -8619,7 +8630,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>61</v>
       </c>
       <c r="B59">
@@ -8633,7 +8644,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>62</v>
       </c>
       <c r="B60">
@@ -8647,7 +8658,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>63</v>
       </c>
       <c r="B61">
@@ -8661,7 +8672,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>64</v>
       </c>
       <c r="B62">
@@ -8675,7 +8686,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>65</v>
       </c>
       <c r="B63">
@@ -8689,7 +8700,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>66</v>
       </c>
       <c r="B64">
@@ -8703,7 +8714,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>67</v>
       </c>
       <c r="B65">
@@ -8717,7 +8728,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>68</v>
       </c>
       <c r="B66">
@@ -8731,7 +8742,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>69</v>
       </c>
       <c r="B67">
@@ -8745,7 +8756,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>70</v>
       </c>
       <c r="B68">
@@ -8759,7 +8770,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>71</v>
       </c>
       <c r="B69">
@@ -8773,7 +8784,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>72</v>
       </c>
       <c r="B70">
@@ -8787,7 +8798,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>73</v>
       </c>
       <c r="B71">
@@ -8801,7 +8812,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>74</v>
       </c>
       <c r="B72">
@@ -8815,7 +8826,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>75</v>
       </c>
       <c r="B73">
@@ -8829,7 +8840,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>76</v>
       </c>
       <c r="B74">
@@ -8843,7 +8854,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>77</v>
       </c>
       <c r="B75">
@@ -8857,7 +8868,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>78</v>
       </c>
       <c r="B76">
@@ -8871,7 +8882,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>79</v>
       </c>
       <c r="B77">
@@ -8885,7 +8896,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>80</v>
       </c>
       <c r="B78">
@@ -8899,7 +8910,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>81</v>
       </c>
       <c r="B79">
@@ -8913,7 +8924,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+      <c r="A80" t="s">
         <v>82</v>
       </c>
       <c r="B80">
@@ -8927,7 +8938,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>83</v>
       </c>
       <c r="B81">
@@ -8941,7 +8952,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>84</v>
       </c>
       <c r="B82">
@@ -8955,7 +8966,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>85</v>
       </c>
       <c r="B83">
@@ -8969,7 +8980,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>86</v>
       </c>
       <c r="B84">
@@ -8983,7 +8994,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>87</v>
       </c>
       <c r="B85">
@@ -8997,7 +9008,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+      <c r="A86" t="s">
         <v>88</v>
       </c>
       <c r="B86">
@@ -9011,7 +9022,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>89</v>
       </c>
       <c r="B87">
@@ -9025,7 +9036,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>90</v>
       </c>
       <c r="B88">
@@ -9039,7 +9050,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>91</v>
       </c>
       <c r="B89">
@@ -9053,7 +9064,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>92</v>
       </c>
       <c r="B90">
@@ -9067,7 +9078,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>93</v>
       </c>
       <c r="B91">
@@ -9081,7 +9092,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>94</v>
       </c>
       <c r="B92">
@@ -9095,7 +9106,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>95</v>
       </c>
       <c r="B93">
@@ -9109,7 +9120,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>96</v>
       </c>
       <c r="B94">
@@ -9123,7 +9134,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>97</v>
       </c>
       <c r="B95">
@@ -9137,7 +9148,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>98</v>
       </c>
       <c r="B96">
@@ -9151,7 +9162,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>99</v>
       </c>
       <c r="B97">
@@ -9165,7 +9176,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
+      <c r="A98" t="s">
         <v>100</v>
       </c>
       <c r="B98">
@@ -9179,7 +9190,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+      <c r="A99" t="s">
         <v>101</v>
       </c>
       <c r="B99">
@@ -9193,7 +9204,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+      <c r="A100" t="s">
         <v>102</v>
       </c>
       <c r="B100">
@@ -9207,7 +9218,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>103</v>
       </c>
       <c r="B101">
@@ -9221,7 +9232,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
+      <c r="A102" t="s">
         <v>104</v>
       </c>
       <c r="B102">
@@ -9235,7 +9246,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+      <c r="A103" t="s">
         <v>105</v>
       </c>
       <c r="B103">
@@ -9249,7 +9260,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+      <c r="A104" t="s">
         <v>106</v>
       </c>
       <c r="B104">
@@ -9263,7 +9274,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
+      <c r="A105" t="s">
         <v>107</v>
       </c>
       <c r="B105">
@@ -9277,7 +9288,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
+      <c r="A106" t="s">
         <v>108</v>
       </c>
       <c r="B106">
@@ -9291,7 +9302,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
+      <c r="A107" t="s">
         <v>109</v>
       </c>
       <c r="B107">
@@ -9305,7 +9316,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+      <c r="A108" t="s">
         <v>110</v>
       </c>
       <c r="B108">
@@ -9319,7 +9330,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+      <c r="A109" t="s">
         <v>111</v>
       </c>
       <c r="B109">
@@ -9333,7 +9344,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+      <c r="A110" t="s">
         <v>112</v>
       </c>
       <c r="B110">
@@ -9347,7 +9358,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>113</v>
       </c>
       <c r="B111">
@@ -9361,7 +9372,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>114</v>
       </c>
       <c r="B112">
@@ -9375,7 +9386,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+      <c r="A113" t="s">
         <v>115</v>
       </c>
       <c r="B113">
@@ -9389,7 +9400,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+      <c r="A114" t="s">
         <v>116</v>
       </c>
       <c r="B114">
@@ -9403,7 +9414,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+      <c r="A115" t="s">
         <v>117</v>
       </c>
       <c r="B115">
@@ -9417,7 +9428,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
+      <c r="A116" t="s">
         <v>118</v>
       </c>
       <c r="B116">
@@ -9431,7 +9442,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+      <c r="A117" t="s">
         <v>119</v>
       </c>
       <c r="B117">
@@ -9445,7 +9456,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>120</v>
       </c>
       <c r="B118">
@@ -9459,7 +9470,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>121</v>
       </c>
       <c r="B119">
@@ -9473,7 +9484,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+      <c r="A120" t="s">
         <v>122</v>
       </c>
       <c r="B120">
@@ -9487,7 +9498,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
+      <c r="A121" t="s">
         <v>123</v>
       </c>
       <c r="B121">
@@ -9501,7 +9512,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
+      <c r="A122" t="s">
         <v>124</v>
       </c>
       <c r="B122">
@@ -9515,7 +9526,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
+      <c r="A123" t="s">
         <v>125</v>
       </c>
       <c r="B123">
@@ -9529,7 +9540,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+      <c r="A124" t="s">
         <v>126</v>
       </c>
       <c r="B124">
@@ -9543,7 +9554,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
+      <c r="A125" t="s">
         <v>127</v>
       </c>
       <c r="B125">
@@ -9557,7 +9568,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
+      <c r="A126" t="s">
         <v>128</v>
       </c>
       <c r="B126">
@@ -9571,7 +9582,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
+      <c r="A127" t="s">
         <v>129</v>
       </c>
       <c r="B127">
@@ -9585,7 +9596,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
+      <c r="A128" t="s">
         <v>130</v>
       </c>
       <c r="B128">
@@ -9599,7 +9610,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
+      <c r="A129" t="s">
         <v>131</v>
       </c>
       <c r="B129">
@@ -9613,7 +9624,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
+      <c r="A130" t="s">
         <v>132</v>
       </c>
       <c r="B130">
@@ -9627,7 +9638,7 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
+      <c r="A131" t="s">
         <v>133</v>
       </c>
       <c r="B131">
@@ -9641,7 +9652,7 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
+      <c r="A132" t="s">
         <v>134</v>
       </c>
       <c r="B132">
@@ -9655,7 +9666,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
+      <c r="A133" t="s">
         <v>135</v>
       </c>
       <c r="B133">
@@ -9669,7 +9680,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
+      <c r="A134" t="s">
         <v>136</v>
       </c>
       <c r="B134">
@@ -9683,7 +9694,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
+      <c r="A135" t="s">
         <v>137</v>
       </c>
       <c r="B135">
@@ -9697,7 +9708,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
+      <c r="A136" t="s">
         <v>138</v>
       </c>
       <c r="B136">
@@ -9711,7 +9722,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
+      <c r="A137" t="s">
         <v>139</v>
       </c>
       <c r="B137">
@@ -9725,7 +9736,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
+      <c r="A138" t="s">
         <v>140</v>
       </c>
       <c r="B138">
@@ -9739,7 +9750,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" s="1" t="s">
+      <c r="A139" t="s">
         <v>141</v>
       </c>
       <c r="B139">
@@ -9753,7 +9764,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" s="1" t="s">
+      <c r="A140" t="s">
         <v>142</v>
       </c>
       <c r="B140">
@@ -9767,7 +9778,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" s="1" t="s">
+      <c r="A141" t="s">
         <v>143</v>
       </c>
       <c r="B141">
@@ -9781,7 +9792,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" s="1" t="s">
+      <c r="A142" t="s">
         <v>144</v>
       </c>
       <c r="B142">
@@ -9795,7 +9806,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" s="1" t="s">
+      <c r="A143" t="s">
         <v>145</v>
       </c>
       <c r="B143">
@@ -9809,7 +9820,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" s="1" t="s">
+      <c r="A144" t="s">
         <v>146</v>
       </c>
       <c r="B144">
@@ -9823,7 +9834,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A145" s="1" t="s">
+      <c r="A145" t="s">
         <v>147</v>
       </c>
       <c r="B145">
@@ -9837,7 +9848,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A146" s="1" t="s">
+      <c r="A146" t="s">
         <v>148</v>
       </c>
       <c r="B146">
@@ -9851,7 +9862,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="1" t="s">
+      <c r="A147" t="s">
         <v>149</v>
       </c>
       <c r="B147">
@@ -9865,7 +9876,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" s="1" t="s">
+      <c r="A148" t="s">
         <v>150</v>
       </c>
       <c r="B148">
@@ -9879,7 +9890,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" s="1" t="s">
+      <c r="A149" t="s">
         <v>151</v>
       </c>
       <c r="B149">
@@ -9893,7 +9904,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" s="1" t="s">
+      <c r="A150" t="s">
         <v>152</v>
       </c>
       <c r="B150">
@@ -9907,7 +9918,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A151" s="1" t="s">
+      <c r="A151" t="s">
         <v>153</v>
       </c>
       <c r="B151">
@@ -9921,7 +9932,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A152" s="1" t="s">
+      <c r="A152" t="s">
         <v>154</v>
       </c>
       <c r="B152">
@@ -9935,7 +9946,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="1" t="s">
+      <c r="A153" t="s">
         <v>155</v>
       </c>
       <c r="B153">
@@ -9949,7 +9960,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" s="1" t="s">
+      <c r="A154" t="s">
         <v>156</v>
       </c>
       <c r="B154">
@@ -9963,7 +9974,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" s="1" t="s">
+      <c r="A155" t="s">
         <v>157</v>
       </c>
       <c r="B155">
@@ -9977,7 +9988,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
+      <c r="A156" t="s">
         <v>158</v>
       </c>
       <c r="B156">
@@ -9991,7 +10002,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="1" t="s">
+      <c r="A157" t="s">
         <v>159</v>
       </c>
       <c r="B157">
@@ -10005,7 +10016,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A158" s="1" t="s">
+      <c r="A158" t="s">
         <v>160</v>
       </c>
       <c r="B158">
@@ -10019,7 +10030,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" s="1" t="s">
+      <c r="A159" t="s">
         <v>161</v>
       </c>
       <c r="B159">
@@ -10033,7 +10044,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="1" t="s">
+      <c r="A160" t="s">
         <v>162</v>
       </c>
       <c r="B160">
@@ -10047,7 +10058,7 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161" s="1" t="s">
+      <c r="A161" t="s">
         <v>163</v>
       </c>
       <c r="B161">
@@ -10061,7 +10072,7 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" s="1" t="s">
+      <c r="A162" t="s">
         <v>164</v>
       </c>
       <c r="B162">
@@ -10075,7 +10086,7 @@
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" s="1" t="s">
+      <c r="A163" t="s">
         <v>165</v>
       </c>
       <c r="B163">
@@ -10089,7 +10100,7 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A164" s="1" t="s">
+      <c r="A164" t="s">
         <v>166</v>
       </c>
       <c r="B164">
@@ -10103,7 +10114,7 @@
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A165" s="1" t="s">
+      <c r="A165" t="s">
         <v>167</v>
       </c>
       <c r="B165">
@@ -10117,7 +10128,7 @@
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A166" s="1" t="s">
+      <c r="A166" t="s">
         <v>168</v>
       </c>
       <c r="B166">
@@ -10131,7 +10142,7 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167" s="1" t="s">
+      <c r="A167" t="s">
         <v>169</v>
       </c>
       <c r="B167">
@@ -10145,7 +10156,7 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A168" s="1" t="s">
+      <c r="A168" t="s">
         <v>170</v>
       </c>
       <c r="B168">
@@ -10159,7 +10170,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" s="1" t="s">
+      <c r="A169" t="s">
         <v>171</v>
       </c>
       <c r="B169">
@@ -10173,7 +10184,7 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170" s="1" t="s">
+      <c r="A170" t="s">
         <v>172</v>
       </c>
       <c r="B170">
@@ -10187,7 +10198,7 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" s="1" t="s">
+      <c r="A171" t="s">
         <v>173</v>
       </c>
       <c r="B171">
@@ -10201,7 +10212,7 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172" s="1" t="s">
+      <c r="A172" t="s">
         <v>174</v>
       </c>
       <c r="B172">
@@ -10215,7 +10226,7 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173" s="1" t="s">
+      <c r="A173" t="s">
         <v>175</v>
       </c>
       <c r="B173">
@@ -10229,7 +10240,7 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A174" s="1" t="s">
+      <c r="A174" t="s">
         <v>176</v>
       </c>
       <c r="B174">
@@ -10243,7 +10254,7 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175" s="1" t="s">
+      <c r="A175" t="s">
         <v>177</v>
       </c>
       <c r="B175">
@@ -10257,7 +10268,7 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A176" s="1" t="s">
+      <c r="A176" t="s">
         <v>178</v>
       </c>
       <c r="B176">
@@ -10271,7 +10282,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A177" s="1" t="s">
+      <c r="A177" t="s">
         <v>179</v>
       </c>
       <c r="B177">
@@ -10285,7 +10296,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A178" s="1" t="s">
+      <c r="A178" t="s">
         <v>180</v>
       </c>
       <c r="B178">
@@ -10299,7 +10310,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A179" s="1" t="s">
+      <c r="A179" t="s">
         <v>181</v>
       </c>
       <c r="B179">
@@ -10313,7 +10324,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" s="1" t="s">
+      <c r="A180" t="s">
         <v>182</v>
       </c>
       <c r="B180">
@@ -10327,7 +10338,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A181" s="1" t="s">
+      <c r="A181" t="s">
         <v>183</v>
       </c>
       <c r="B181">
@@ -10341,7 +10352,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A182" s="1" t="s">
+      <c r="A182" t="s">
         <v>184</v>
       </c>
       <c r="B182">
@@ -10355,7 +10366,7 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A183" s="1" t="s">
+      <c r="A183" t="s">
         <v>185</v>
       </c>
       <c r="B183">
@@ -10369,7 +10380,7 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A184" s="1" t="s">
+      <c r="A184" t="s">
         <v>186</v>
       </c>
       <c r="B184">
@@ -10383,7 +10394,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A185" s="1" t="s">
+      <c r="A185" t="s">
         <v>187</v>
       </c>
       <c r="B185">
@@ -10397,7 +10408,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A186" s="1" t="s">
+      <c r="A186" t="s">
         <v>188</v>
       </c>
       <c r="B186">
@@ -10411,7 +10422,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A187" s="1" t="s">
+      <c r="A187" t="s">
         <v>189</v>
       </c>
       <c r="B187">
@@ -10425,7 +10436,7 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A188" s="1" t="s">
+      <c r="A188" t="s">
         <v>190</v>
       </c>
       <c r="B188">
@@ -10439,7 +10450,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A189" s="1" t="s">
+      <c r="A189" t="s">
         <v>191</v>
       </c>
       <c r="B189">
@@ -10453,7 +10464,7 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" s="1" t="s">
+      <c r="A190" t="s">
         <v>192</v>
       </c>
       <c r="B190">
@@ -10467,7 +10478,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191" s="1" t="s">
+      <c r="A191" t="s">
         <v>193</v>
       </c>
       <c r="B191">
@@ -10481,7 +10492,7 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" s="1" t="s">
+      <c r="A192" t="s">
         <v>194</v>
       </c>
       <c r="B192">
@@ -10495,7 +10506,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193" s="1" t="s">
+      <c r="A193" t="s">
         <v>195</v>
       </c>
       <c r="B193">
@@ -10509,7 +10520,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A194" s="1" t="s">
+      <c r="A194" t="s">
         <v>196</v>
       </c>
       <c r="B194">
@@ -10523,7 +10534,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A195" s="1" t="s">
+      <c r="A195" t="s">
         <v>197</v>
       </c>
       <c r="B195">
@@ -10537,7 +10548,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A196" s="1" t="s">
+      <c r="A196" t="s">
         <v>198</v>
       </c>
       <c r="B196">
@@ -10551,7 +10562,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A197" s="1" t="s">
+      <c r="A197" t="s">
         <v>199</v>
       </c>
       <c r="B197">
@@ -10565,7 +10576,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" s="1" t="s">
+      <c r="A198" t="s">
         <v>200</v>
       </c>
       <c r="B198">
@@ -10579,7 +10590,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A199" s="1" t="s">
+      <c r="A199" t="s">
         <v>201</v>
       </c>
       <c r="B199">
@@ -10593,7 +10604,7 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A200" s="1" t="s">
+      <c r="A200" t="s">
         <v>202</v>
       </c>
       <c r="B200">
@@ -10607,7 +10618,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A201" s="1" t="s">
+      <c r="A201" t="s">
         <v>203</v>
       </c>
       <c r="B201">
@@ -10621,7 +10632,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A202" s="1" t="s">
+      <c r="A202" t="s">
         <v>204</v>
       </c>
       <c r="B202">
@@ -10635,7 +10646,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A203" s="1" t="s">
+      <c r="A203" t="s">
         <v>205</v>
       </c>
       <c r="B203">
@@ -10649,7 +10660,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A204" s="1" t="s">
+      <c r="A204" t="s">
         <v>206</v>
       </c>
       <c r="B204">
@@ -10663,7 +10674,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A205" s="1" t="s">
+      <c r="A205" t="s">
         <v>207</v>
       </c>
       <c r="B205">
@@ -10677,7 +10688,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A206" s="1" t="s">
+      <c r="A206" t="s">
         <v>208</v>
       </c>
       <c r="B206">
@@ -10691,7 +10702,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A207" s="1" t="s">
+      <c r="A207" t="s">
         <v>209</v>
       </c>
       <c r="B207">
@@ -10705,7 +10716,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A208" s="1" t="s">
+      <c r="A208" t="s">
         <v>210</v>
       </c>
       <c r="B208">
@@ -10719,7 +10730,7 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A209" s="1" t="s">
+      <c r="A209" t="s">
         <v>211</v>
       </c>
       <c r="B209">
@@ -10733,7 +10744,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A210" s="1" t="s">
+      <c r="A210" t="s">
         <v>212</v>
       </c>
       <c r="B210">
@@ -10747,7 +10758,7 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A211" s="1" t="s">
+      <c r="A211" t="s">
         <v>213</v>
       </c>
       <c r="B211">
@@ -10761,7 +10772,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A212" s="1" t="s">
+      <c r="A212" t="s">
         <v>214</v>
       </c>
       <c r="B212">
@@ -10775,7 +10786,7 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A213" s="1" t="s">
+      <c r="A213" t="s">
         <v>215</v>
       </c>
       <c r="B213">
@@ -10789,7 +10800,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A214" s="1" t="s">
+      <c r="A214" t="s">
         <v>216</v>
       </c>
       <c r="B214">
@@ -10803,7 +10814,7 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A215" s="1" t="s">
+      <c r="A215" t="s">
         <v>217</v>
       </c>
       <c r="B215">
@@ -10817,7 +10828,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A216" s="1" t="s">
+      <c r="A216" t="s">
         <v>218</v>
       </c>
       <c r="B216">
@@ -10831,7 +10842,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A217" s="1" t="s">
+      <c r="A217" t="s">
         <v>219</v>
       </c>
       <c r="B217">
@@ -10845,7 +10856,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A218" s="1" t="s">
+      <c r="A218" t="s">
         <v>220</v>
       </c>
       <c r="B218">
@@ -10859,7 +10870,7 @@
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A219" s="1" t="s">
+      <c r="A219" t="s">
         <v>221</v>
       </c>
       <c r="B219">
@@ -10873,7 +10884,7 @@
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A220" s="1" t="s">
+      <c r="A220" t="s">
         <v>222</v>
       </c>
       <c r="B220">
@@ -10887,7 +10898,7 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A221" s="1" t="s">
+      <c r="A221" t="s">
         <v>223</v>
       </c>
       <c r="B221">
@@ -10901,7 +10912,7 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A222" s="1" t="s">
+      <c r="A222" t="s">
         <v>224</v>
       </c>
       <c r="B222">
@@ -10915,7 +10926,7 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A223" s="1" t="s">
+      <c r="A223" t="s">
         <v>225</v>
       </c>
       <c r="B223">
@@ -10929,7 +10940,7 @@
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A224" s="1" t="s">
+      <c r="A224" t="s">
         <v>226</v>
       </c>
       <c r="B224">
@@ -10943,7 +10954,7 @@
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A225" s="1" t="s">
+      <c r="A225" t="s">
         <v>227</v>
       </c>
       <c r="B225">
@@ -10957,7 +10968,7 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A226" s="1" t="s">
+      <c r="A226" t="s">
         <v>228</v>
       </c>
       <c r="B226">
@@ -10971,7 +10982,7 @@
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A227" s="1" t="s">
+      <c r="A227" t="s">
         <v>229</v>
       </c>
       <c r="B227">
@@ -10985,7 +10996,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A228" s="1" t="s">
+      <c r="A228" t="s">
         <v>230</v>
       </c>
       <c r="B228">
@@ -10999,7 +11010,7 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A229" s="1" t="s">
+      <c r="A229" t="s">
         <v>231</v>
       </c>
       <c r="B229">
@@ -11013,7 +11024,7 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A230" s="1" t="s">
+      <c r="A230" t="s">
         <v>232</v>
       </c>
       <c r="B230">
@@ -11027,7 +11038,7 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A231" s="1" t="s">
+      <c r="A231" t="s">
         <v>233</v>
       </c>
       <c r="B231">
@@ -11041,7 +11052,7 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A232" s="1" t="s">
+      <c r="A232" t="s">
         <v>234</v>
       </c>
       <c r="B232">
@@ -11055,7 +11066,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A233" s="1" t="s">
+      <c r="A233" t="s">
         <v>235</v>
       </c>
       <c r="B233">
@@ -11069,7 +11080,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A234" s="1" t="s">
+      <c r="A234" t="s">
         <v>236</v>
       </c>
       <c r="B234">
@@ -11083,7 +11094,7 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A235" s="1" t="s">
+      <c r="A235" t="s">
         <v>237</v>
       </c>
       <c r="B235">
@@ -11097,7 +11108,7 @@
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A236" s="1" t="s">
+      <c r="A236" t="s">
         <v>238</v>
       </c>
       <c r="B236">
@@ -11111,7 +11122,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A237" s="1" t="s">
+      <c r="A237" t="s">
         <v>239</v>
       </c>
       <c r="B237">
@@ -11125,7 +11136,7 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A238" s="1" t="s">
+      <c r="A238" t="s">
         <v>240</v>
       </c>
       <c r="B238">
@@ -11139,7 +11150,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A239" s="1" t="s">
+      <c r="A239" t="s">
         <v>241</v>
       </c>
       <c r="B239">
@@ -11153,7 +11164,7 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A240" s="1" t="s">
+      <c r="A240" t="s">
         <v>242</v>
       </c>
       <c r="B240">
@@ -11167,7 +11178,7 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A241" s="1" t="s">
+      <c r="A241" t="s">
         <v>243</v>
       </c>
       <c r="B241">
@@ -11181,7 +11192,7 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A242" s="1" t="s">
+      <c r="A242" t="s">
         <v>244</v>
       </c>
       <c r="B242">
@@ -11195,7 +11206,7 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A243" s="1" t="s">
+      <c r="A243" t="s">
         <v>245</v>
       </c>
       <c r="B243">
@@ -11209,7 +11220,7 @@
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A244" s="1" t="s">
+      <c r="A244" t="s">
         <v>246</v>
       </c>
       <c r="B244">
@@ -11223,7 +11234,7 @@
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A245" s="1" t="s">
+      <c r="A245" t="s">
         <v>247</v>
       </c>
       <c r="B245">
@@ -11237,7 +11248,7 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A246" s="1" t="s">
+      <c r="A246" t="s">
         <v>248</v>
       </c>
       <c r="B246">
@@ -11251,7 +11262,7 @@
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A247" s="1" t="s">
+      <c r="A247" t="s">
         <v>249</v>
       </c>
       <c r="B247">
@@ -11265,7 +11276,7 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A248" s="1" t="s">
+      <c r="A248" t="s">
         <v>250</v>
       </c>
       <c r="B248">
@@ -11279,7 +11290,7 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A249" s="1" t="s">
+      <c r="A249" t="s">
         <v>251</v>
       </c>
       <c r="B249">
@@ -11293,7 +11304,7 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A250" s="1" t="s">
+      <c r="A250" t="s">
         <v>252</v>
       </c>
       <c r="B250">
@@ -11307,7 +11318,7 @@
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A251" s="1" t="s">
+      <c r="A251" t="s">
         <v>253</v>
       </c>
       <c r="B251">
@@ -11321,7 +11332,7 @@
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A252" s="1" t="s">
+      <c r="A252" t="s">
         <v>254</v>
       </c>
       <c r="B252">
@@ -11335,7 +11346,7 @@
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A253" s="1" t="s">
+      <c r="A253" t="s">
         <v>255</v>
       </c>
       <c r="B253">
@@ -11349,7 +11360,7 @@
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A254" s="1" t="s">
+      <c r="A254" t="s">
         <v>256</v>
       </c>
       <c r="B254">
@@ -11363,7 +11374,7 @@
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A255" s="1" t="s">
+      <c r="A255" t="s">
         <v>257</v>
       </c>
       <c r="B255">
@@ -11377,7 +11388,7 @@
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A256" s="1" t="s">
+      <c r="A256" t="s">
         <v>258</v>
       </c>
       <c r="B256">
@@ -11391,7 +11402,7 @@
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A257" s="1" t="s">
+      <c r="A257" t="s">
         <v>259</v>
       </c>
       <c r="B257">
@@ -11405,7 +11416,7 @@
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A258" s="1" t="s">
+      <c r="A258" t="s">
         <v>260</v>
       </c>
       <c r="B258">
@@ -11419,7 +11430,7 @@
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A259" s="1" t="s">
+      <c r="A259" t="s">
         <v>261</v>
       </c>
       <c r="B259">
@@ -11433,7 +11444,7 @@
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A260" s="1" t="s">
+      <c r="A260" t="s">
         <v>262</v>
       </c>
       <c r="B260">
@@ -11447,7 +11458,7 @@
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A261" s="1" t="s">
+      <c r="A261" t="s">
         <v>263</v>
       </c>
       <c r="B261">
@@ -11461,7 +11472,7 @@
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A262" s="1" t="s">
+      <c r="A262" t="s">
         <v>264</v>
       </c>
       <c r="B262">
@@ -11475,7 +11486,7 @@
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A263" s="1" t="s">
+      <c r="A263" t="s">
         <v>265</v>
       </c>
       <c r="B263">
@@ -11489,7 +11500,7 @@
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A264" s="1" t="s">
+      <c r="A264" t="s">
         <v>266</v>
       </c>
       <c r="B264">
@@ -11503,7 +11514,7 @@
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A265" s="1" t="s">
+      <c r="A265" t="s">
         <v>267</v>
       </c>
       <c r="B265">
@@ -11517,7 +11528,7 @@
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A266" s="1" t="s">
+      <c r="A266" t="s">
         <v>268</v>
       </c>
       <c r="B266">
@@ -11531,7 +11542,7 @@
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A267" s="1" t="s">
+      <c r="A267" t="s">
         <v>269</v>
       </c>
       <c r="B267">
@@ -11545,7 +11556,7 @@
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A268" s="1" t="s">
+      <c r="A268" t="s">
         <v>270</v>
       </c>
       <c r="B268">
@@ -11559,7 +11570,7 @@
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A269" s="1" t="s">
+      <c r="A269" t="s">
         <v>271</v>
       </c>
       <c r="B269">
@@ -11573,7 +11584,7 @@
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A270" s="1" t="s">
+      <c r="A270" t="s">
         <v>272</v>
       </c>
       <c r="B270">
@@ -11587,7 +11598,7 @@
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A271" s="1" t="s">
+      <c r="A271" t="s">
         <v>273</v>
       </c>
       <c r="B271">
@@ -11601,7 +11612,7 @@
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A272" s="1" t="s">
+      <c r="A272" t="s">
         <v>274</v>
       </c>
       <c r="B272">
@@ -11615,7 +11626,7 @@
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A273" s="1" t="s">
+      <c r="A273" t="s">
         <v>275</v>
       </c>
       <c r="B273">
@@ -11629,7 +11640,7 @@
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A274" s="1" t="s">
+      <c r="A274" t="s">
         <v>276</v>
       </c>
       <c r="B274">
@@ -11643,7 +11654,7 @@
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A275" s="1" t="s">
+      <c r="A275" t="s">
         <v>277</v>
       </c>
       <c r="B275">
@@ -11657,7 +11668,7 @@
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A276" s="1" t="s">
+      <c r="A276" t="s">
         <v>278</v>
       </c>
       <c r="B276">
@@ -11671,7 +11682,7 @@
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A277" s="1" t="s">
+      <c r="A277" t="s">
         <v>279</v>
       </c>
       <c r="B277">
@@ -11685,7 +11696,7 @@
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A278" s="1" t="s">
+      <c r="A278" t="s">
         <v>280</v>
       </c>
       <c r="B278">
@@ -11699,7 +11710,7 @@
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A279" s="1" t="s">
+      <c r="A279" t="s">
         <v>281</v>
       </c>
       <c r="B279">
@@ -11713,7 +11724,7 @@
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A280" s="1" t="s">
+      <c r="A280" t="s">
         <v>282</v>
       </c>
       <c r="B280">
@@ -11727,7 +11738,7 @@
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A281" s="1" t="s">
+      <c r="A281" t="s">
         <v>283</v>
       </c>
       <c r="B281">
@@ -11741,7 +11752,7 @@
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A282" s="1" t="s">
+      <c r="A282" t="s">
         <v>284</v>
       </c>
       <c r="B282">
@@ -11755,7 +11766,7 @@
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A283" s="1" t="s">
+      <c r="A283" t="s">
         <v>285</v>
       </c>
       <c r="B283">
@@ -11769,7 +11780,7 @@
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A284" s="1" t="s">
+      <c r="A284" t="s">
         <v>286</v>
       </c>
       <c r="B284">
@@ -11783,7 +11794,7 @@
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A285" s="1" t="s">
+      <c r="A285" t="s">
         <v>287</v>
       </c>
       <c r="B285">
@@ -11797,7 +11808,7 @@
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A286" s="1" t="s">
+      <c r="A286" t="s">
         <v>288</v>
       </c>
       <c r="B286">
@@ -11811,7 +11822,7 @@
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A287" s="1" t="s">
+      <c r="A287" t="s">
         <v>289</v>
       </c>
       <c r="B287">
@@ -11825,7 +11836,7 @@
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A288" s="1" t="s">
+      <c r="A288" t="s">
         <v>290</v>
       </c>
       <c r="B288">
@@ -11839,7 +11850,7 @@
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A289" s="1" t="s">
+      <c r="A289" t="s">
         <v>291</v>
       </c>
       <c r="B289">
@@ -11853,7 +11864,7 @@
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A290" s="1" t="s">
+      <c r="A290" t="s">
         <v>292</v>
       </c>
       <c r="B290">
@@ -11867,7 +11878,7 @@
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A291" s="1" t="s">
+      <c r="A291" t="s">
         <v>293</v>
       </c>
       <c r="B291">
@@ -11881,7 +11892,7 @@
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A292" s="1" t="s">
+      <c r="A292" t="s">
         <v>294</v>
       </c>
       <c r="B292">
@@ -11895,7 +11906,7 @@
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A293" s="1" t="s">
+      <c r="A293" t="s">
         <v>295</v>
       </c>
       <c r="B293">
@@ -11909,7 +11920,7 @@
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A294" s="1" t="s">
+      <c r="A294" t="s">
         <v>296</v>
       </c>
       <c r="B294">
@@ -11923,7 +11934,7 @@
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A295" s="1" t="s">
+      <c r="A295" t="s">
         <v>297</v>
       </c>
       <c r="B295">
@@ -11937,7 +11948,7 @@
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A296" s="1" t="s">
+      <c r="A296" t="s">
         <v>298</v>
       </c>
       <c r="B296">
@@ -11951,7 +11962,7 @@
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A297" s="1" t="s">
+      <c r="A297" t="s">
         <v>299</v>
       </c>
       <c r="B297">
@@ -11965,7 +11976,7 @@
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A298" s="1" t="s">
+      <c r="A298" t="s">
         <v>300</v>
       </c>
       <c r="B298">
@@ -11979,7 +11990,7 @@
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A299" s="1" t="s">
+      <c r="A299" t="s">
         <v>301</v>
       </c>
       <c r="B299">
@@ -11993,7 +12004,7 @@
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A300" s="1" t="s">
+      <c r="A300" t="s">
         <v>302</v>
       </c>
       <c r="B300">
@@ -12007,7 +12018,7 @@
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A301" s="1" t="s">
+      <c r="A301" t="s">
         <v>303</v>
       </c>
       <c r="B301">
@@ -12021,7 +12032,7 @@
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A302" s="1" t="s">
+      <c r="A302" t="s">
         <v>304</v>
       </c>
       <c r="B302">
@@ -12035,7 +12046,7 @@
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A303" s="1" t="s">
+      <c r="A303" t="s">
         <v>305</v>
       </c>
       <c r="B303">
@@ -12049,7 +12060,7 @@
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A304" s="1" t="s">
+      <c r="A304" t="s">
         <v>306</v>
       </c>
       <c r="B304">
@@ -12063,7 +12074,7 @@
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A305" s="1" t="s">
+      <c r="A305" t="s">
         <v>307</v>
       </c>
       <c r="B305">
@@ -12077,7 +12088,7 @@
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A306" s="1" t="s">
+      <c r="A306" t="s">
         <v>308</v>
       </c>
       <c r="B306">
@@ -12091,7 +12102,7 @@
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A307" s="1" t="s">
+      <c r="A307" t="s">
         <v>309</v>
       </c>
       <c r="B307">
@@ -12105,7 +12116,7 @@
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A308" s="1" t="s">
+      <c r="A308" t="s">
         <v>310</v>
       </c>
       <c r="B308">
@@ -12119,7 +12130,7 @@
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A309" s="1" t="s">
+      <c r="A309" t="s">
         <v>311</v>
       </c>
       <c r="B309">
@@ -12133,7 +12144,7 @@
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A310" s="1" t="s">
+      <c r="A310" t="s">
         <v>312</v>
       </c>
       <c r="B310">
@@ -12147,7 +12158,7 @@
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A311" s="1" t="s">
+      <c r="A311" t="s">
         <v>313</v>
       </c>
       <c r="B311">
@@ -12161,7 +12172,7 @@
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A312" s="1" t="s">
+      <c r="A312" t="s">
         <v>314</v>
       </c>
       <c r="B312">
@@ -12175,7 +12186,7 @@
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A313" s="1" t="s">
+      <c r="A313" t="s">
         <v>315</v>
       </c>
       <c r="B313">
@@ -12189,7 +12200,7 @@
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A314" s="1" t="s">
+      <c r="A314" t="s">
         <v>316</v>
       </c>
       <c r="B314">
@@ -12203,7 +12214,7 @@
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A315" s="1" t="s">
+      <c r="A315" t="s">
         <v>317</v>
       </c>
       <c r="B315">
@@ -12217,7 +12228,7 @@
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A316" s="1" t="s">
+      <c r="A316" t="s">
         <v>318</v>
       </c>
       <c r="B316">
@@ -12231,7 +12242,7 @@
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A317" s="1" t="s">
+      <c r="A317" t="s">
         <v>319</v>
       </c>
       <c r="B317">
@@ -12245,7 +12256,7 @@
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A318" s="1" t="s">
+      <c r="A318" t="s">
         <v>320</v>
       </c>
       <c r="B318">
@@ -12259,7 +12270,7 @@
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A319" s="1" t="s">
+      <c r="A319" t="s">
         <v>321</v>
       </c>
       <c r="B319">
@@ -12273,7 +12284,7 @@
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A320" s="1" t="s">
+      <c r="A320" t="s">
         <v>322</v>
       </c>
       <c r="B320">
@@ -12287,7 +12298,7 @@
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A321" s="1" t="s">
+      <c r="A321" t="s">
         <v>323</v>
       </c>
       <c r="B321">
@@ -12301,7 +12312,7 @@
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A322" s="1" t="s">
+      <c r="A322" t="s">
         <v>324</v>
       </c>
       <c r="B322">
@@ -12315,7 +12326,7 @@
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A323" s="1" t="s">
+      <c r="A323" t="s">
         <v>325</v>
       </c>
       <c r="B323">
@@ -12329,7 +12340,7 @@
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A324" s="1" t="s">
+      <c r="A324" t="s">
         <v>326</v>
       </c>
       <c r="B324">
@@ -12343,7 +12354,7 @@
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A325" s="1" t="s">
+      <c r="A325" t="s">
         <v>327</v>
       </c>
       <c r="B325">
@@ -12357,7 +12368,7 @@
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A326" s="1" t="s">
+      <c r="A326" t="s">
         <v>328</v>
       </c>
       <c r="B326">
@@ -12371,7 +12382,7 @@
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A327" s="1" t="s">
+      <c r="A327" t="s">
         <v>329</v>
       </c>
       <c r="B327">
@@ -12385,7 +12396,7 @@
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A328" s="1" t="s">
+      <c r="A328" t="s">
         <v>330</v>
       </c>
       <c r="B328">
@@ -12399,7 +12410,7 @@
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A329" s="1" t="s">
+      <c r="A329" t="s">
         <v>331</v>
       </c>
       <c r="B329">
@@ -12413,7 +12424,7 @@
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A330" s="1" t="s">
+      <c r="A330" t="s">
         <v>332</v>
       </c>
       <c r="B330">
@@ -12427,7 +12438,7 @@
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A331" s="1" t="s">
+      <c r="A331" t="s">
         <v>333</v>
       </c>
       <c r="B331">
@@ -12441,7 +12452,7 @@
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A332" s="1" t="s">
+      <c r="A332" t="s">
         <v>334</v>
       </c>
       <c r="B332">
@@ -12455,7 +12466,7 @@
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A333" s="1" t="s">
+      <c r="A333" t="s">
         <v>335</v>
       </c>
       <c r="B333">
@@ -12469,7 +12480,7 @@
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A334" s="1" t="s">
+      <c r="A334" t="s">
         <v>336</v>
       </c>
       <c r="B334">
@@ -12483,7 +12494,7 @@
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A335" s="1" t="s">
+      <c r="A335" t="s">
         <v>337</v>
       </c>
       <c r="B335">
@@ -12497,7 +12508,7 @@
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A336" s="1" t="s">
+      <c r="A336" t="s">
         <v>338</v>
       </c>
       <c r="B336">
@@ -12511,7 +12522,7 @@
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A337" s="1" t="s">
+      <c r="A337" t="s">
         <v>339</v>
       </c>
       <c r="B337">
@@ -12525,7 +12536,7 @@
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A338" s="1" t="s">
+      <c r="A338" t="s">
         <v>340</v>
       </c>
       <c r="B338">
@@ -12539,7 +12550,7 @@
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A339" s="1" t="s">
+      <c r="A339" t="s">
         <v>341</v>
       </c>
       <c r="B339">
@@ -12553,7 +12564,7 @@
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A340" s="1" t="s">
+      <c r="A340" t="s">
         <v>342</v>
       </c>
       <c r="B340">
@@ -12567,7 +12578,7 @@
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A341" s="1" t="s">
+      <c r="A341" t="s">
         <v>343</v>
       </c>
       <c r="B341">
@@ -12581,7 +12592,7 @@
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A342" s="1" t="s">
+      <c r="A342" t="s">
         <v>344</v>
       </c>
       <c r="B342">
@@ -12595,7 +12606,7 @@
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A343" s="1" t="s">
+      <c r="A343" t="s">
         <v>345</v>
       </c>
       <c r="B343">
@@ -12609,7 +12620,7 @@
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A344" s="1" t="s">
+      <c r="A344" t="s">
         <v>346</v>
       </c>
       <c r="B344">
@@ -12623,7 +12634,7 @@
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A345" s="1" t="s">
+      <c r="A345" t="s">
         <v>347</v>
       </c>
       <c r="B345">
@@ -12637,7 +12648,7 @@
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A346" s="1" t="s">
+      <c r="A346" t="s">
         <v>348</v>
       </c>
       <c r="B346">
@@ -12651,7 +12662,7 @@
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A347" s="1" t="s">
+      <c r="A347" t="s">
         <v>349</v>
       </c>
       <c r="B347">
@@ -12665,7 +12676,7 @@
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A348" s="1" t="s">
+      <c r="A348" t="s">
         <v>350</v>
       </c>
       <c r="B348">
@@ -12679,7 +12690,7 @@
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A349" s="1" t="s">
+      <c r="A349" t="s">
         <v>351</v>
       </c>
       <c r="B349">
@@ -12693,7 +12704,7 @@
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A350" s="1" t="s">
+      <c r="A350" t="s">
         <v>352</v>
       </c>
       <c r="B350">
@@ -12707,7 +12718,7 @@
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A351" s="1" t="s">
+      <c r="A351" t="s">
         <v>353</v>
       </c>
       <c r="B351">
@@ -12721,7 +12732,7 @@
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A352" s="1" t="s">
+      <c r="A352" t="s">
         <v>354</v>
       </c>
       <c r="B352">

</xml_diff>